<commit_message>
data semua santri dan tulisan mading
</commit_message>
<xml_diff>
--- a/pesantren/data mabaiz/data semua santri.xlsx
+++ b/pesantren/data mabaiz/data semua santri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZEN-PROJECT\zen\pesantren\data mabaiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5152D8B5-B499-4076-A975-194D76845439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909DDC5F-2918-4AF4-84D4-60D2FACFF2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="1560" windowWidth="13185" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="593">
   <si>
     <t>nama santri</t>
   </si>
@@ -1608,145 +1608,211 @@
     <t>082148689206</t>
   </si>
   <si>
+    <t>Samarinda, 18 Juni 2011</t>
+  </si>
+  <si>
+    <t>Jalan Gelatik 1, Blok B, RT 13, No 9, Kelurahan Temindung Permai, Kecamatan Sungai Pinang, Samarinda, Kalimantan Timur</t>
+  </si>
+  <si>
+    <t>Staf TU</t>
+  </si>
+  <si>
+    <t>085246205524</t>
+  </si>
+  <si>
+    <t>6472085806110002</t>
+  </si>
+  <si>
+    <t>Samarinda, 22 Februari 2011</t>
+  </si>
+  <si>
+    <t>Jalan Jenderal Urip Sumoharjo, Gang Lestari, No 5, RT 28</t>
+  </si>
+  <si>
+    <t>Andriadi</t>
+  </si>
+  <si>
+    <t>082350416888</t>
+  </si>
+  <si>
+    <t>Herlina</t>
+  </si>
+  <si>
+    <t>081250259199</t>
+  </si>
+  <si>
+    <t>6472042202110004</t>
+  </si>
+  <si>
+    <t>Samarinda, 12 Mei 2011</t>
+  </si>
+  <si>
+    <t>Desa Senyiur</t>
+  </si>
+  <si>
+    <t>Edi Rachman</t>
+  </si>
+  <si>
+    <t>081351407060</t>
+  </si>
+  <si>
+    <t>Yunita Vitaloka</t>
+  </si>
+  <si>
+    <t>081351254741</t>
+  </si>
+  <si>
+    <t>6408011205110001</t>
+  </si>
+  <si>
+    <t>Samarinda, 28 April 2011</t>
+  </si>
+  <si>
+    <t>Jalan Cipto Mangunkusumo, RT 9, Sengkotek, Loa Janan Ilir, Samarinda</t>
+  </si>
+  <si>
+    <t>Roni Muharsyah</t>
+  </si>
+  <si>
+    <t>081515877493</t>
+  </si>
+  <si>
+    <t>Sari Kurniawati</t>
+  </si>
+  <si>
+    <t>6402036604110001</t>
+  </si>
+  <si>
+    <t>Wildan Akhram Pratama</t>
+  </si>
+  <si>
+    <t>23.02.071</t>
+  </si>
+  <si>
+    <t>Samarinda, 28 Maret 2010</t>
+  </si>
+  <si>
+    <t>Simpang Tiga, Loa Janan Ilir, RT 10</t>
+  </si>
+  <si>
+    <t>Suparji</t>
+  </si>
+  <si>
+    <t>081347716701</t>
+  </si>
+  <si>
+    <t>Sukatmi</t>
+  </si>
+  <si>
+    <t>6472025304990003</t>
+  </si>
+  <si>
+    <t>081222240832</t>
+  </si>
+  <si>
+    <t>6472031103110001</t>
+  </si>
+  <si>
+    <t>Samarinda, 11 Maret 2011</t>
+  </si>
+  <si>
+    <t>Samarinda, 28 September 2011</t>
+  </si>
+  <si>
+    <t>Perumahan Pondok Karya Lestari, Blok D, No 39, RT 15, Kelurahan Sungai Kapih, Kecamatan Sambutan, Samarinda, Kalimantan Timur</t>
+  </si>
+  <si>
+    <t>M Agus Kastiawan</t>
+  </si>
+  <si>
+    <t>Guru ASN</t>
+  </si>
+  <si>
+    <t>Halimatus Sa'diyah</t>
+  </si>
+  <si>
+    <t>085250464198</t>
+  </si>
+  <si>
+    <t>6472056809110001</t>
+  </si>
+  <si>
+    <t>nisn</t>
+  </si>
+  <si>
+    <t>nis</t>
+  </si>
+  <si>
+    <t>Hazwan Hafizuddin</t>
+  </si>
+  <si>
+    <t>6402034307100001</t>
+  </si>
+  <si>
+    <t>6472061111090006</t>
+  </si>
+  <si>
+    <t>6472073101100002</t>
+  </si>
+  <si>
+    <t>6472030210100002</t>
+  </si>
+  <si>
+    <t>6472050403100005</t>
+  </si>
+  <si>
+    <t>6472020805090003</t>
+  </si>
+  <si>
+    <t>6402036308090003</t>
+  </si>
+  <si>
+    <t>6472067112090002</t>
+  </si>
+  <si>
+    <t>6472052802100001</t>
+  </si>
+  <si>
+    <t>6472024108090003</t>
+  </si>
+  <si>
+    <t>6472052112080004</t>
+  </si>
+  <si>
+    <t>6402161504090001</t>
+  </si>
+  <si>
+    <t>6402060410080002</t>
+  </si>
+  <si>
+    <t>6472031901080002</t>
+  </si>
+  <si>
+    <t>6402036011080002</t>
+  </si>
+  <si>
+    <t>6402044505090002</t>
+  </si>
+  <si>
+    <t>6472036612000004</t>
+  </si>
+  <si>
+    <t>6402037006080005</t>
+  </si>
+  <si>
+    <t>3315081502080001</t>
+  </si>
+  <si>
+    <t>3518135304000002</t>
+  </si>
+  <si>
     <t>6402131606100002</t>
   </si>
   <si>
-    <t>Samarinda, 18 Juni 2011</t>
-  </si>
-  <si>
-    <t>Jalan Gelatik 1, Blok B, RT 13, No 9, Kelurahan Temindung Permai, Kecamatan Sungai Pinang, Samarinda, Kalimantan Timur</t>
-  </si>
-  <si>
-    <t>Staf TU</t>
-  </si>
-  <si>
-    <t>085246205524</t>
-  </si>
-  <si>
-    <t>6472085806110002</t>
-  </si>
-  <si>
-    <t>Samarinda, 22 Februari 2011</t>
-  </si>
-  <si>
-    <t>Jalan Jenderal Urip Sumoharjo, Gang Lestari, No 5, RT 28</t>
-  </si>
-  <si>
-    <t>Andriadi</t>
-  </si>
-  <si>
-    <t>082350416888</t>
-  </si>
-  <si>
-    <t>Herlina</t>
-  </si>
-  <si>
-    <t>081250259199</t>
-  </si>
-  <si>
-    <t>6472042202110004</t>
-  </si>
-  <si>
-    <t>Samarinda, 12 Mei 2011</t>
-  </si>
-  <si>
-    <t>Desa Senyiur</t>
-  </si>
-  <si>
-    <t>Edi Rachman</t>
-  </si>
-  <si>
-    <t>081351407060</t>
-  </si>
-  <si>
-    <t>Yunita Vitaloka</t>
-  </si>
-  <si>
-    <t>081351254741</t>
-  </si>
-  <si>
-    <t>6408011205110001</t>
-  </si>
-  <si>
-    <t>Samarinda, 28 April 2011</t>
-  </si>
-  <si>
-    <t>Jalan Cipto Mangunkusumo, RT 9, Sengkotek, Loa Janan Ilir, Samarinda</t>
-  </si>
-  <si>
-    <t>Roni Muharsyah</t>
-  </si>
-  <si>
-    <t>081515877493</t>
-  </si>
-  <si>
-    <t>Sari Kurniawati</t>
-  </si>
-  <si>
-    <t>6402036604110001</t>
-  </si>
-  <si>
-    <t>Wildan Akhram Pratama</t>
-  </si>
-  <si>
-    <t>23.02.071</t>
-  </si>
-  <si>
-    <t>Samarinda, 28 Maret 2010</t>
-  </si>
-  <si>
-    <t>Simpang Tiga, Loa Janan Ilir, RT 10</t>
-  </si>
-  <si>
-    <t>Suparji</t>
-  </si>
-  <si>
-    <t>081347716701</t>
-  </si>
-  <si>
-    <t>Sukatmi</t>
-  </si>
-  <si>
-    <t>6472025304990003</t>
-  </si>
-  <si>
-    <t>081222240832</t>
-  </si>
-  <si>
-    <t>6472031103110001</t>
-  </si>
-  <si>
-    <t>Samarinda, 11 Maret 2011</t>
-  </si>
-  <si>
-    <t>Samarinda, 28 September 2011</t>
-  </si>
-  <si>
-    <t>Perumahan Pondok Karya Lestari, Blok D, No 39, RT 15, Kelurahan Sungai Kapih, Kecamatan Sambutan, Samarinda, Kalimantan Timur</t>
-  </si>
-  <si>
-    <t>M Agus Kastiawan</t>
-  </si>
-  <si>
-    <t>Guru ASN</t>
-  </si>
-  <si>
-    <t>Halimatus Sa'diyah</t>
-  </si>
-  <si>
-    <t>085250464198</t>
-  </si>
-  <si>
-    <t>6472056809110001</t>
-  </si>
-  <si>
-    <t>nisn</t>
-  </si>
-  <si>
-    <t>nis</t>
-  </si>
-  <si>
-    <t>Hazwan Hafizuddin</t>
+    <t>6402162605090001</t>
+  </si>
+  <si>
+    <t>6472052305090001</t>
   </si>
 </sst>
 </file>
@@ -1934,7 +2000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2024,11 +2090,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2307,9 +2376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7A9B44-12F6-4712-8C6B-1EA7374A630C}">
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2343,10 +2412,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>567</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>568</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>569</v>
       </c>
       <c r="D1" s="43" t="s">
         <v>3</v>
@@ -2472,7 +2541,7 @@
         <v>393</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>37</v>
@@ -2484,29 +2553,29 @@
         <v>23</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I3" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Perumahan Pondok Karya Lestari, Blok D, No 39, RT 15, Kelurahan Sungai Kapih, Kecamatan Sambutan, Samarinda, Kalimantan Timur</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>125</v>
       </c>
       <c r="L3" s="34" t="s">
+        <v>563</v>
+      </c>
+      <c r="M3" s="34" t="s">
         <v>564</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="N3" s="35" t="s">
         <v>565</v>
       </c>
-      <c r="N3" s="35" t="s">
-        <v>566</v>
-      </c>
       <c r="O3" s="34" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="P3" s="44" t="s">
         <v>29</v>
@@ -2520,7 +2589,7 @@
       <c r="S3" s="34"/>
       <c r="T3" s="34"/>
       <c r="U3" s="35" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -2650,7 +2719,7 @@
         <v>396</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>37</v>
@@ -2662,7 +2731,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I6" s="34" t="str">
         <f t="shared" si="0"/>
@@ -2675,13 +2744,13 @@
         <v>98</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M6" s="34" t="s">
         <v>103</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="O6" s="34" t="s">
         <v>129</v>
@@ -2698,7 +2767,7 @@
       <c r="S6" s="34"/>
       <c r="T6" s="34"/>
       <c r="U6" s="35" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -2768,7 +2837,7 @@
         <v>398</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>37</v>
@@ -2780,23 +2849,23 @@
         <v>23</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I8" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Jalan Cipto Mangunkusumo, RT 9, Sengkotek, Loa Janan Ilir, Samarinda</v>
       </c>
       <c r="J8" s="34" t="s">
+        <v>545</v>
+      </c>
+      <c r="K8" s="35" t="s">
         <v>546</v>
-      </c>
-      <c r="K8" s="35" t="s">
-        <v>547</v>
       </c>
       <c r="L8" s="34" t="s">
         <v>40</v>
       </c>
       <c r="M8" s="34" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="N8" s="34" t="str">
         <f>K8</f>
@@ -2815,7 +2884,7 @@
       <c r="S8" s="34"/>
       <c r="T8" s="34"/>
       <c r="U8" s="35" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -2827,7 +2896,7 @@
         <v>399</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>426</v>
@@ -2839,23 +2908,23 @@
         <v>23</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I9" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Simpang Tiga, Loa Janan Ilir, RT 10</v>
       </c>
       <c r="J9" s="34" t="s">
+        <v>553</v>
+      </c>
+      <c r="K9" s="35" t="s">
         <v>554</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>555</v>
       </c>
       <c r="L9" s="34" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N9" s="34"/>
       <c r="O9" s="34" t="s">
@@ -2873,7 +2942,7 @@
       <c r="S9" s="35"/>
       <c r="T9" s="35"/>
       <c r="U9" s="35" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2885,7 +2954,7 @@
         <v>400</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>426</v>
@@ -2916,7 +2985,7 @@
         <v>271</v>
       </c>
       <c r="N10" s="35" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="O10" s="34" t="s">
         <v>40</v>
@@ -2933,11 +3002,11 @@
       <c r="S10" s="35"/>
       <c r="T10" s="35"/>
       <c r="U10" s="35" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="51" t="s">
         <v>383</v>
       </c>
       <c r="B11" s="18"/>
@@ -3139,7 +3208,7 @@
         <v>405</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>426</v>
@@ -3151,26 +3220,26 @@
         <v>23</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I15" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Jalan Jenderal Urip Sumoharjo, Gang Lestari, No 5, RT 28</v>
       </c>
       <c r="J15" s="34" t="s">
+        <v>531</v>
+      </c>
+      <c r="K15" s="35" t="s">
         <v>532</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>533</v>
       </c>
       <c r="L15" s="34" t="s">
         <v>327</v>
       </c>
       <c r="M15" s="34" t="s">
+        <v>533</v>
+      </c>
+      <c r="N15" s="35" t="s">
         <v>534</v>
-      </c>
-      <c r="N15" s="35" t="s">
-        <v>535</v>
       </c>
       <c r="O15" s="34" t="s">
         <v>28</v>
@@ -3187,7 +3256,7 @@
       <c r="S15" s="35"/>
       <c r="T15" s="35"/>
       <c r="U15" s="35" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3199,7 +3268,7 @@
         <v>406</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>426</v>
@@ -3211,26 +3280,26 @@
         <v>23</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I16" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Desa Senyiur</v>
       </c>
       <c r="J16" s="34" t="s">
+        <v>538</v>
+      </c>
+      <c r="K16" s="35" t="s">
         <v>539</v>
-      </c>
-      <c r="K16" s="35" t="s">
-        <v>540</v>
       </c>
       <c r="L16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="M16" s="34" t="s">
+        <v>540</v>
+      </c>
+      <c r="N16" s="35" t="s">
         <v>541</v>
-      </c>
-      <c r="N16" s="35" t="s">
-        <v>542</v>
       </c>
       <c r="O16" s="34" t="s">
         <v>28</v>
@@ -3247,7 +3316,7 @@
       <c r="S16" s="35"/>
       <c r="T16" s="35"/>
       <c r="U16" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3429,7 +3498,7 @@
       </c>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="51" t="s">
         <v>374</v>
       </c>
       <c r="B20" s="32"/>
@@ -3523,16 +3592,16 @@
       <c r="S21" s="35"/>
       <c r="T21" s="35"/>
       <c r="U21" s="35" t="s">
-        <v>524</v>
+        <v>590</v>
       </c>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="49" t="s">
-        <v>550</v>
+      <c r="A22" s="51" t="s">
+        <v>549</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -3606,7 +3675,7 @@
       <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="49" t="s">
         <v>473</v>
       </c>
       <c r="B32" s="31"/>
@@ -3618,7 +3687,7 @@
       <c r="B33" s="28"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="49" t="s">
         <v>475</v>
       </c>
       <c r="B34" s="31"/>
@@ -3642,7 +3711,7 @@
       <c r="B37" s="31"/>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="49" t="s">
         <v>479</v>
       </c>
       <c r="B38" s="31"/>
@@ -3654,7 +3723,7 @@
       <c r="B39" s="31"/>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="49" t="s">
         <v>481</v>
       </c>
       <c r="B40" s="31"/>
@@ -3678,7 +3747,7 @@
       <c r="B43" s="31"/>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="50" t="s">
+      <c r="A44" s="49" t="s">
         <v>485</v>
       </c>
       <c r="B44" s="30"/>
@@ -3696,9 +3765,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3838,6 +3907,9 @@
       <c r="R2" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S2" s="12" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="10" t="s">
@@ -3895,6 +3967,9 @@
       <c r="R3" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S3" s="12" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="10" t="s">
@@ -4009,6 +4084,9 @@
       <c r="R5" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S5" s="12" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="10" t="s">
@@ -4066,6 +4144,9 @@
       <c r="R6" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S6" s="12" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="10" t="s">
@@ -4123,6 +4204,9 @@
       <c r="R7" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S7" s="12" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="10" t="s">
@@ -4180,6 +4264,9 @@
       <c r="R8" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S8" s="12" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="10" t="s">
@@ -4237,6 +4324,9 @@
       <c r="R9" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S9" s="12" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="8" t="s">
@@ -4294,6 +4384,9 @@
       <c r="R10" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S10" s="12" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="10" t="s">
@@ -4351,6 +4444,9 @@
       <c r="R11" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="S11" s="12" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="10" t="s">
@@ -4407,6 +4503,9 @@
       </c>
       <c r="R12" s="12" t="s">
         <v>32</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15.75">
@@ -4450,12 +4549,12 @@
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="49" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="49" t="s">
         <v>462</v>
       </c>
     </row>
@@ -4465,7 +4564,7 @@
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="49" t="s">
         <v>464</v>
       </c>
     </row>
@@ -4487,8 +4586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4744,7 +4843,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="46" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>131</v>
@@ -5826,34 +5925,52 @@
       <c r="A25" s="45" t="s">
         <v>442</v>
       </c>
+      <c r="B25" s="16" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="50" t="s">
         <v>443</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="45" t="s">
         <v>444</v>
       </c>
+      <c r="B27" s="16" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="23" t="s">
         <v>445</v>
       </c>
+      <c r="B28" s="16" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="23" t="s">
         <v>446</v>
       </c>
+      <c r="B29" s="16" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="50" t="s">
         <v>447</v>
       </c>
+      <c r="B30" s="16" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="50" t="s">
         <v>448</v>
       </c>
     </row>
@@ -5861,32 +5978,50 @@
       <c r="A32" s="23" t="s">
         <v>449</v>
       </c>
+      <c r="B32" s="16" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="23" t="s">
         <v>450</v>
       </c>
+      <c r="B33" s="16" t="s">
+        <v>589</v>
+      </c>
       <c r="H33" s="25"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="23" t="s">
         <v>451</v>
       </c>
+      <c r="B34" s="16" t="s">
+        <v>585</v>
+      </c>
       <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="23" t="s">
         <v>452</v>
       </c>
+      <c r="B35" s="16" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="23" t="s">
         <v>453</v>
       </c>
+      <c r="B36" s="16" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="26" t="s">
         <v>454</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="41" spans="1:8">

</xml_diff>